<commit_message>
update flowchart and eval results
</commit_message>
<xml_diff>
--- a/eval/evaluation.xlsx
+++ b/eval/evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tianyu Wang\Documents\Notebooks\EnhancedCyberSecEd-LLMs\eval\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E209C202-522F-48EA-A30B-A10D304AA3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A2C82-116A-46AD-94FF-32B25160700C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4455" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="10" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="563">
   <si>
     <t>input_question</t>
   </si>
@@ -3951,6 +3951,39 @@
   </si>
   <si>
     <t>helpfulness</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Cybersecurity</t>
+  </si>
+  <si>
+    <t>Cryptography</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t># of Question</t>
+  </si>
+  <si>
+    <t>Helpfulness</t>
+  </si>
+  <si>
+    <t>Correctness</t>
+  </si>
+  <si>
+    <t>Completeness</t>
+  </si>
+  <si>
+    <t>115 (Total)</t>
+  </si>
+  <si>
+    <t>completeness</t>
+  </si>
+  <si>
+    <t>avg (coding)</t>
   </si>
 </sst>
 </file>
@@ -4467,7 +4500,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4512,6 +4545,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4870,10 +4921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD86063-7ACE-46E3-965F-7EBC46B0038B}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4888,25 +4939,51 @@
     <col min="8" max="9" width="11.3828125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.4609375" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.3828125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.23046875" style="5"/>
+    <col min="12" max="12" width="10.765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.23046875" style="5"/>
+    <col min="14" max="14" width="12.07421875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.69140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16.07421875" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.4609375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.23046875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A1" s="16" t="s">
-        <v>550</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
+        <v>551</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="N1" s="19" t="s">
+        <v>552</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>556</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="S1"/>
+      <c r="T1"/>
+      <c r="U1"/>
+      <c r="V1"/>
+      <c r="W1"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>549</v>
       </c>
@@ -4914,6 +4991,7 @@
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="14" t="s">
         <v>548</v>
       </c>
@@ -4921,8 +4999,28 @@
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
       <c r="K2" s="14"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="N2" s="18" t="s">
+        <v>553</v>
+      </c>
+      <c r="O2" s="18">
+        <v>75</v>
+      </c>
+      <c r="P2" s="22">
+        <v>0.94</v>
+      </c>
+      <c r="Q2" s="22">
+        <v>0.91</v>
+      </c>
+      <c r="R2" s="22">
+        <v>0.87</v>
+      </c>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+    </row>
+    <row r="3" spans="1:23" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="6" t="s">
         <v>442</v>
       </c>
@@ -4953,178 +5051,301 @@
       <c r="K3" s="6" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L3" s="6" t="s">
+        <v>562</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>554</v>
+      </c>
+      <c r="O3" s="18">
+        <v>10</v>
+      </c>
+      <c r="P3" s="22">
+        <v>0.87</v>
+      </c>
+      <c r="Q3" s="22">
+        <v>0.63</v>
+      </c>
+      <c r="R3" s="22">
+        <v>0.89</v>
+      </c>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>443</v>
       </c>
       <c r="B4" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="C4" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="10">
+        <v>0.99</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="5">
         <v>1</v>
       </c>
-      <c r="E4" s="10">
-        <v>0.8</v>
+      <c r="E4" s="5">
+        <v>0.7</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="5">
+        <v>0.97</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="5">
         <v>0.95</v>
       </c>
-      <c r="I4" s="10">
+      <c r="K4" s="5">
         <v>0.7</v>
       </c>
-      <c r="J4" s="10">
-        <v>0.95</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="N4" s="18" t="s">
+        <v>555</v>
+      </c>
+      <c r="O4" s="18">
+        <v>30</v>
+      </c>
+      <c r="P4" s="22">
+        <v>0.8</v>
+      </c>
+      <c r="Q4" s="22">
+        <v>0.89</v>
+      </c>
+      <c r="R4" s="22">
+        <v>0.92</v>
+      </c>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+    </row>
+    <row r="5" spans="1:23" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>444</v>
       </c>
       <c r="B5" s="5">
-        <v>0.96</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="D5" s="10">
-        <v>0.85</v>
-      </c>
-      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
         <v>0.8</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.3</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="H5" s="10">
-        <v>0.89</v>
-      </c>
-      <c r="I5" s="10">
+      <c r="H5" s="5">
+        <v>0.93</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="K5" s="5">
         <v>0.6</v>
       </c>
-      <c r="J5" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="K5" s="10">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="N5" s="9"/>
+      <c r="O5" s="18" t="s">
+        <v>560</v>
+      </c>
+      <c r="P5" s="23">
+        <f>AVERAGE(P2:P4)</f>
+        <v>0.87000000000000011</v>
+      </c>
+      <c r="Q5" s="23">
+        <f t="shared" ref="Q5:R5" si="0">AVERAGE(Q2:Q4)</f>
+        <v>0.81</v>
+      </c>
+      <c r="R5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.89333333333333342</v>
+      </c>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>445</v>
       </c>
       <c r="B6" s="5">
-        <v>0.96</v>
-      </c>
-      <c r="C6" s="10">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
         <v>0.5</v>
-      </c>
-      <c r="D6" s="10">
-        <v>0.95</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0.9</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="H6" s="10">
-        <v>0.89</v>
-      </c>
-      <c r="I6" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="J6" s="10">
-        <v>1</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="H6" s="5">
+        <v>0.92</v>
+      </c>
+      <c r="I6" s="5">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J6" s="5">
+        <v>0.95</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="B7" s="11">
-        <f t="shared" ref="B7:E7" si="0">AVERAGE(B4:B6)</f>
-        <v>0.96333333333333326</v>
+      <c r="B7" s="10">
+        <f>AVERAGE(B4:B6)</f>
+        <v>0.9966666666666667</v>
       </c>
       <c r="C7" s="10">
-        <f t="shared" si="0"/>
-        <v>0.53333333333333333</v>
+        <f t="shared" ref="C7:E7" si="1">AVERAGE(C4:C6)</f>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D7" s="10">
-        <f>AVERAGE(D4:D6)</f>
-        <v>0.93333333333333324</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="E7" s="10">
-        <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
+        <f t="shared" si="1"/>
+        <v>0.5</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="H7" s="11">
-        <f t="shared" ref="H7:K7" si="1">AVERAGE(H4:H6)</f>
-        <v>0.91</v>
+      <c r="H7" s="10">
+        <f>AVERAGE(H4:H6)</f>
+        <v>0.94</v>
       </c>
       <c r="I7" s="10">
-        <f t="shared" si="1"/>
-        <v>0.6333333333333333</v>
+        <f t="shared" ref="I7:K7" si="2">AVERAGE(I4:I6)</f>
+        <v>0.8666666666666667</v>
       </c>
       <c r="J7" s="10">
-        <f>AVERAGE(J4:J6)</f>
-        <v>0.95000000000000007</v>
+        <f t="shared" si="2"/>
+        <v>0.93333333333333324</v>
       </c>
       <c r="K7" s="10">
-        <f t="shared" si="1"/>
-        <v>0.83333333333333337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="L7" s="10">
+        <f>AVERAGE(J7:K7)</f>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A8" s="6" t="s">
         <v>518</v>
       </c>
       <c r="B8" s="12">
         <f>AVERAGE(B7:E7)</f>
-        <v>0.8158333333333333</v>
+        <v>0.83250000000000002</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>518</v>
       </c>
       <c r="H8" s="12">
         <f>AVERAGE(H7:K7)</f>
-        <v>0.83166666666666678</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A11" s="17" t="s">
-        <v>551</v>
-      </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.85166666666666657</v>
+      </c>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.4">
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+    </row>
+    <row r="11" spans="1:23" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="N11" s="21"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A12" s="14" t="s">
         <v>549</v>
       </c>
@@ -5132,7 +5353,6 @@
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
-      <c r="F12" s="9"/>
       <c r="G12" s="14" t="s">
         <v>548</v>
       </c>
@@ -5140,8 +5360,18 @@
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
       <c r="K12" s="14"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="N12" s="21"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A13" s="6" t="s">
         <v>442</v>
       </c>
@@ -5172,162 +5402,172 @@
       <c r="K13" s="6" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L13" s="6" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>443</v>
       </c>
       <c r="B14" s="5">
-        <v>0.99</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="D14" s="5">
+        <v>0.97</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D14" s="10">
         <v>1</v>
       </c>
-      <c r="E14" s="5">
-        <v>0.7</v>
+      <c r="E14" s="10">
+        <v>0.8</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>443</v>
       </c>
-      <c r="H14" s="5">
-        <v>0.97</v>
-      </c>
-      <c r="I14" s="5">
-        <v>1</v>
-      </c>
-      <c r="J14" s="5">
+      <c r="H14" s="10">
         <v>0.95</v>
       </c>
-      <c r="K14" s="5">
+      <c r="I14" s="10">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="J14" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>444</v>
       </c>
       <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="5">
+        <v>0.96</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="E15" s="10">
         <v>0.8</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0.3</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>444</v>
       </c>
-      <c r="H15" s="5">
-        <v>0.93</v>
-      </c>
-      <c r="I15" s="5">
+      <c r="H15" s="10">
+        <v>0.89</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="K15" s="10">
         <v>0.8</v>
       </c>
-      <c r="J15" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>445</v>
       </c>
       <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-      <c r="E16" s="5">
+        <v>0.96</v>
+      </c>
+      <c r="C16" s="10">
         <v>0.5</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.9</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>445</v>
       </c>
-      <c r="H16" s="5">
-        <v>0.92</v>
-      </c>
-      <c r="I16" s="5">
+      <c r="H16" s="10">
+        <v>0.89</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="J16" s="10">
+        <v>1</v>
+      </c>
+      <c r="K16" s="10">
         <v>0.8</v>
       </c>
-      <c r="J16" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="K16" s="5">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="11">
         <f>AVERAGE(B14:B16)</f>
-        <v>0.9966666666666667</v>
+        <v>0.96333333333333326</v>
       </c>
       <c r="C17" s="10">
-        <f t="shared" ref="C17:E17" si="2">AVERAGE(C14:C16)</f>
+        <f>AVERAGE(C14:C16)</f>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="D17" s="10">
+        <f>AVERAGE(D14:D16)</f>
+        <v>0.93333333333333324</v>
+      </c>
+      <c r="E17" s="10">
+        <f>AVERAGE(E14:E16)</f>
         <v>0.83333333333333337</v>
-      </c>
-      <c r="D17" s="10">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E17" s="10">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="11">
         <f>AVERAGE(H14:H16)</f>
-        <v>0.94</v>
+        <v>0.91</v>
       </c>
       <c r="I17" s="10">
-        <f t="shared" ref="I17:K17" si="3">AVERAGE(I14:I16)</f>
-        <v>0.8666666666666667</v>
+        <f>AVERAGE(I14:I16)</f>
+        <v>0.6333333333333333</v>
       </c>
       <c r="J17" s="10">
-        <f t="shared" si="3"/>
-        <v>0.93333333333333324</v>
+        <f>AVERAGE(J14:J16)</f>
+        <v>0.95000000000000007</v>
       </c>
       <c r="K17" s="10">
-        <f t="shared" si="3"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+        <f>AVERAGE(K14:K16)</f>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="L17" s="10">
+        <f>AVERAGE(J17:K17)</f>
+        <v>0.89166666666666672</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A18" s="6" t="s">
         <v>518</v>
       </c>
       <c r="B18" s="12">
         <f>AVERAGE(B17:E17)</f>
-        <v>0.83250000000000002</v>
+        <v>0.8158333333333333</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>518</v>
       </c>
       <c r="H18" s="12">
         <f>AVERAGE(H17:K17)</f>
-        <v>0.85166666666666657</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+        <v>0.83166666666666678</v>
+      </c>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A20" s="15" t="s">
-        <v>551</v>
+        <v>561</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
@@ -5340,7 +5580,7 @@
       <c r="J20" s="15"/>
       <c r="K20" s="15"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G21" s="14" t="s">
         <v>548</v>
       </c>
@@ -5349,7 +5589,7 @@
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G22" s="6" t="s">
         <v>442</v>
       </c>
@@ -5365,8 +5605,11 @@
       <c r="K22" s="6" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L22" s="6" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G23" s="5" t="s">
         <v>328</v>
       </c>
@@ -5382,8 +5625,12 @@
       <c r="K23" s="13">
         <v>0.90661643305830897</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L23" s="10">
+        <f>AVERAGE(J23:K23)</f>
+        <v>0.91979809898960241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.4">
       <c r="G24" s="6" t="s">
         <v>518</v>
       </c>
@@ -5396,14 +5643,15 @@
   <mergeCells count="8">
     <mergeCell ref="G21:K21"/>
     <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A11:K11"/>
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A11:K11"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="G12:K12"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="G12:K12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>